<commit_message>
Exercícios de DML e DQL concluídos
</commit_message>
<xml_diff>
--- a/Exercícios - Modelagens/1.4 - Música/resolucao_1-4_fisico.xlsx
+++ b/Exercícios - Modelagens/1.4 - Música/resolucao_1-4_fisico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinixiii\Desktop\2DM-S1-banco-de-dados\Exercícios - Modelagens\1.4 - Música\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE564F0-C88F-40B9-8AD0-B27BD65B3C2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FAA26A-E37E-4DEB-9D1B-3558B25B797B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{560FD7A5-98CB-4676-A41C-6B22AD31494D}"/>
+    <workbookView xWindow="5805" yWindow="4020" windowWidth="21600" windowHeight="11385" xr2:uid="{560FD7A5-98CB-4676-A41C-6B22AD31494D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha3" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Nome</t>
   </si>
@@ -90,18 +90,9 @@
     <t>IdEstilos</t>
   </si>
   <si>
-    <t>Acesso</t>
-  </si>
-  <si>
     <t>IdStatus</t>
   </si>
   <si>
-    <t>Ativo</t>
-  </si>
-  <si>
-    <t>Inativo</t>
-  </si>
-  <si>
     <t>IdUsuario</t>
   </si>
   <si>
@@ -160,6 +151,12 @@
   </si>
   <si>
     <t>Pagode</t>
+  </si>
+  <si>
+    <t>Disponível</t>
+  </si>
+  <si>
+    <t>Indisponível</t>
   </si>
 </sst>
 </file>
@@ -189,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +214,66 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,7 +344,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -308,25 +365,60 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -645,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F263AA-B3AF-49DC-BC15-D984EE5D7C9E}">
-  <dimension ref="B2:AF7"/>
+  <dimension ref="B2:AC7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:O2"/>
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,168 +750,157 @@
     <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="10.85546875" customWidth="1"/>
-    <col min="30" max="30" width="7" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="10.85546875" customWidth="1"/>
+    <col min="27" max="27" width="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.28515625" customWidth="1"/>
-    <col min="41" max="41" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.28515625" customWidth="1"/>
+    <col min="38" max="38" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.7109375" customWidth="1"/>
+    <col min="41" max="41" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="9.7109375" customWidth="1"/>
     <col min="44" max="44" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.7109375" customWidth="1"/>
-    <col min="47" max="47" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="E2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="12"/>
+      <c r="K2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="14"/>
+      <c r="N2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="17"/>
+      <c r="Q2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="Y2" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z2" s="23"/>
+      <c r="AB2" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="26"/>
+    </row>
+    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="E2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="10"/>
-      <c r="K2" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="14"/>
-      <c r="N2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="O2" s="14"/>
-      <c r="Q2" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="14"/>
-      <c r="T2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AB2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC2" s="14"/>
-      <c r="AE2" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF2" s="14"/>
-    </row>
-    <row r="3" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="E3" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="W3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y3" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z3" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB3" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC3" s="27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="W3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="H4" s="1">
         <v>123</v>
@@ -830,61 +911,55 @@
       <c r="K4" s="1">
         <v>1</v>
       </c>
-      <c r="L4" s="1">
-        <v>1</v>
+      <c r="L4" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="N4" s="1">
         <v>1</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="Q4" s="1">
         <v>1</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="R4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S4" s="5">
+        <v>44249</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="T4" s="1">
-        <v>1</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V4" s="5">
-        <v>44249</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X4" s="1">
+      <c r="U4" s="1">
         <v>30</v>
       </c>
-      <c r="Y4" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>1</v>
+      <c r="V4" s="1">
+        <v>1</v>
+      </c>
+      <c r="W4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>3</v>
       </c>
       <c r="AB4" s="3">
         <v>1</v>
       </c>
-      <c r="AC4" s="3">
-        <v>3</v>
-      </c>
-      <c r="AE4" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="2" t="s">
+      <c r="AC4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
@@ -892,8 +967,8 @@
       <c r="F5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>35</v>
+      <c r="G5" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="H5" s="1">
         <v>1234</v>
@@ -902,66 +977,60 @@
         <v>2</v>
       </c>
       <c r="K5" s="1">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="N5" s="1">
         <v>2</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="Q5" s="1">
         <v>2</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="R5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S5" s="5">
+        <v>44250</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="T5" s="1">
-        <v>2</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="V5" s="5">
-        <v>44250</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X5" s="1">
+      <c r="U5" s="1">
         <v>30</v>
       </c>
-      <c r="Y5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="1">
+      <c r="V5" s="1">
+        <v>1</v>
+      </c>
+      <c r="W5" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="3">
         <v>2</v>
       </c>
       <c r="AB5" s="3">
         <v>2</v>
       </c>
-      <c r="AC5" s="3">
-        <v>2</v>
-      </c>
-      <c r="AE5" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF5" s="2" t="s">
+      <c r="AC5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="E6" s="1">
         <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>34</v>
+      <c r="G6" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="H6" s="1">
         <v>12345</v>
@@ -969,71 +1038,64 @@
       <c r="I6" s="1">
         <v>2</v>
       </c>
-      <c r="K6" s="1">
-        <v>2</v>
-      </c>
-      <c r="L6" s="1">
-        <v>1</v>
+      <c r="N6" s="1">
+        <v>3</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="Q6" s="1">
         <v>3</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="R6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S6" s="5">
+        <v>44251</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="T6" s="1">
+      <c r="U6" s="1">
+        <v>30</v>
+      </c>
+      <c r="V6" s="1">
+        <v>2</v>
+      </c>
+      <c r="W6" s="1">
         <v>3</v>
       </c>
-      <c r="U6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V6" s="5">
-        <v>44251</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="X6" s="1">
-        <v>30</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>2</v>
-      </c>
-      <c r="Z6" s="1">
+      <c r="Y6" s="3">
         <v>3</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>1</v>
       </c>
       <c r="AB6" s="3">
         <v>3</v>
       </c>
-      <c r="AC6" s="3">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="3">
+      <c r="AC6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Y7" s="3">
         <v>3</v>
       </c>
-      <c r="AF6" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="AB7" s="3">
-        <v>3</v>
-      </c>
-      <c r="AC7" s="3">
-        <v>2</v>
-      </c>
-      <c r="AE7" s="4"/>
+      <c r="Z7" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
+    <mergeCell ref="Q2:W2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="N2:O2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="T2:Z2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AE2:AF2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>